<commit_message>
Old Selenium scripts added
</commit_message>
<xml_diff>
--- a/Selenium_Java_Framework/excelfiles/TestData.xlsx
+++ b/Selenium_Java_Framework/excelfiles/TestData.xlsx
@@ -3,22 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anki\git\TestRepo\Selenium_Java_Framework\excelfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC2BFE0-ABAC-46C9-969F-6FBC36B2B593}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D097344-A2DE-4F0B-9C4D-7C53FCA6FF6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="RegData" sheetId="2" r:id="rId2"/>
+    <sheet name="LoginData" r:id="rId6" sheetId="3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Username</t>
   </si>
@@ -95,12 +96,25 @@
   </si>
   <si>
     <t>shreyash123</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>Admin123</t>
+  </si>
+  <si>
+    <t>admin11</t>
+  </si>
+  <si>
+    <t>status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -126,12 +140,52 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -147,10 +201,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -487,10 +545,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -558,4 +616,53 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.2265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.62109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="3">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>